<commit_message>
Se finalizan transacciones Sprint 5
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/generarclave/generar_clave.xlsx
+++ b/SVP/src/test/resources/datadriven/generarclave/generar_clave.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26311"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TESTBDD\SVP_NEW\SVP\src\test\resources\datadriven\autenticacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/svp-rediseno-personas-web-tests-bdd-screenplay/SVP/src/test/resources/datadriven/generarclave/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14760" windowHeight="6495"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
     <sheet name="Listas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Orientacion</t>
   </si>
@@ -33,9 +36,6 @@
     <t>Acierto</t>
   </si>
   <si>
-    <t>000</t>
-  </si>
-  <si>
     <t>tipoDocumento</t>
   </si>
   <si>
@@ -69,56 +69,14 @@
     <t>usuario</t>
   </si>
   <si>
-    <t>0369</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Alterno</t>
-  </si>
-  <si>
-    <t>CLAVE NO VALIDA</t>
-  </si>
-  <si>
-    <t>052</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>607</t>
-  </si>
-  <si>
-    <t>CLAVE BLOQUEADA</t>
-  </si>
-  <si>
-    <t>1373022</t>
-  </si>
-  <si>
-    <t>usua22rio</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>2443</t>
-  </si>
-  <si>
-    <t>1373023</t>
-  </si>
-  <si>
-    <t>1373024</t>
-  </si>
-  <si>
-    <t>Inicio2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,16 +120,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,153 +464,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -664,7 +542,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B4</xm:sqref>
+          <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -678,21 +556,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se termina transaccion Generar Clave y se modifica autenticacion
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/generarclave/generar_clave.xlsx
+++ b/SVP/src/test/resources/datadriven/generarclave/generar_clave.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Orientacion</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Alterno</t>
+  </si>
+  <si>
+    <t>mensajeEsperado</t>
+  </si>
+  <si>
+    <t>La nueva clave quedará pendiente de activación en la Sucursal Física. Si eres colombiano en el exterior comunícate con la Sucursal Telefónica.</t>
   </si>
 </sst>
 </file>
@@ -110,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -133,11 +139,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -150,6 +167,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -484,7 +504,7 @@
     <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -515,8 +535,11 @@
       <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="K1" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -531,6 +554,9 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="4"/>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se crean escenarios adicionales para generar clave
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/generarclave/generar_clave.xlsx
+++ b/SVP/src/test/resources/datadriven/generarclave/generar_clave.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t xml:space="preserve">idCaso</t>
   </si>
@@ -59,25 +59,55 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
+    <t xml:space="preserve">Alterno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario o clave inválida. Inténtalo nuevamente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1001945795</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chipote95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cédula de ciudadanía</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Acierto</t>
   </si>
   <si>
+    <t xml:space="preserve">1245123880</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OSVPPRU96</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Debes activar la clave en la Sucursal Física. Si eres colombiano en el exterior comunícate con la Sucursal Telefónica.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
     <t xml:space="preserve">25130110</t>
   </si>
   <si>
     <t xml:space="preserve">USUCDTC1</t>
   </si>
   <si>
-    <t xml:space="preserve">Cédula de ciudadanía</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Debes activar la clave en la Sucursal Física. Si eres colombiano en el exterior comunícate con la Sucursal Telefónica.</t>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La clave que usas en el cajero está bloqueada. Debes activarla en la Sucursal Física. Para mayor información comunícate con la Sucursal Telefónica.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
   </si>
   <si>
     <t xml:space="preserve">Orientacion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alterno</t>
   </si>
 </sst>
 </file>
@@ -187,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -213,6 +243,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,13 +327,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.14"/>
@@ -348,7 +382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -357,29 +391,126 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="6" t="n">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>4321</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="6" t="n">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="6" t="n">
+        <v>1234</v>
+      </c>
+      <c r="I3" s="6" t="n">
+        <v>1234</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="6" t="n">
         <v>4321</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I4" s="6" t="n">
         <v>1234</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="0" t="s">
+      <c r="J4" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="K4" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B6" type="list">
       <formula1>Listas!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -405,21 +536,21 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adecuancion escenario bloqueo por svp
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/generarclave/generar_clave.xlsx
+++ b/SVP/src/test/resources/datadriven/generarclave/generar_clave.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t xml:space="preserve">idCaso</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1002576587</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chipote87</t>
   </si>
   <si>
     <t xml:space="preserve">Orientacion</t>
@@ -118,7 +124,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -147,6 +153,12 @@
       <name val="Mic Shell Dlg"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -217,7 +229,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -248,6 +260,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -330,10 +346,10 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.14"/>
@@ -502,11 +518,21 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="4"/>
+      <c r="F6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <v>4321</v>
+      </c>
+      <c r="I6" s="6" t="n">
+        <v>4321</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -536,11 +562,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Se agrega escenario documento no existente para generar clave
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/generarclave/generar_clave.xlsx
+++ b/SVP/src/test/resources/datadriven/generarclave/generar_clave.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t xml:space="preserve">idCaso</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t xml:space="preserve">chipote87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12343565433322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">docnoexiste</t>
   </si>
   <si>
     <t xml:space="preserve">Orientacion</t>
@@ -229,7 +238,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -264,6 +273,10 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -343,13 +356,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.14"/>
@@ -530,13 +543,44 @@
       <c r="I6" s="6" t="n">
         <v>4321</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="4" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <v>4321</v>
+      </c>
+      <c r="I7" s="6" t="n">
+        <v>4321</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B6" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B7" type="list">
       <formula1>Listas!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -562,11 +606,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>